<commit_message>
added the pip files
</commit_message>
<xml_diff>
--- a/data/Fakedata.xlsx
+++ b/data/Fakedata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianmasse/Developer/Classes/CSC630/group-work/Commons-Data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840110BB-2973-334F-9BE1-BE76143AA11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0CB225-4120-E948-A56A-221E0EFDE3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="2140" windowWidth="29940" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="C1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="I1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>

</xml_diff>